<commit_message>
update why we sleep
</commit_message>
<xml_diff>
--- a/time records/record.xlsx
+++ b/time records/record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kth-my.sharepoint.com/personal/yangch_ug_kth_se/Documents/PhD/study notes/daily writing/time records/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="160" documentId="8_{EB022E86-9F53-3749-8E02-F1EB961DD2B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F6DA818-299F-FA45-81B1-221693AB4FFA}"/>
+  <xr:revisionPtr revIDLastSave="181" documentId="8_{EB022E86-9F53-3749-8E02-F1EB961DD2B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31593102-1B1A-644B-B619-A1D5290E7E3C}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="580" windowWidth="26740" windowHeight="16380" xr2:uid="{75E0E992-E93C-194B-84F3-B52702DB8E82}"/>
+    <workbookView xWindow="0" yWindow="1580" windowWidth="27040" windowHeight="15980" xr2:uid="{75E0E992-E93C-194B-84F3-B52702DB8E82}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
   <si>
     <t>日期</t>
   </si>
@@ -146,10 +146,16 @@
     <t>睡觉</t>
   </si>
   <si>
-    <t xml:space="preserve">todo: swish, 热菜不粘锅 </t>
-  </si>
-  <si>
     <t>当尼采哭泣 1-8章</t>
+  </si>
+  <si>
+    <t>为什么睡觉</t>
+  </si>
+  <si>
+    <t>todo: swish</t>
+  </si>
+  <si>
+    <t>起床</t>
   </si>
 </sst>
 </file>
@@ -511,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71202AD9-F6AE-7E4C-A4C7-3746B5A46B93}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -790,7 +796,7 @@
         <v>60</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -865,7 +871,7 @@
         <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D28" s="2">
         <v>182</v>
@@ -900,15 +906,75 @@
       <c r="A31" s="1">
         <v>44948</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
-        <v>44948</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>44948</v>
+        <v>44949</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>44949</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>44949</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>44949</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>44949</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>44949</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>44949</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>44949</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update Nietzsche git push
</commit_message>
<xml_diff>
--- a/time records/record.xlsx
+++ b/time records/record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kth-my.sharepoint.com/personal/yangch_ug_kth_se/Documents/PhD/study notes/daily writing/time records/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="205" documentId="8_{EB022E86-9F53-3749-8E02-F1EB961DD2B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F11E6A60-CC7F-C74E-B170-04001524B211}"/>
+  <xr:revisionPtr revIDLastSave="283" documentId="8_{EB022E86-9F53-3749-8E02-F1EB961DD2B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C2918C1-C0D9-3040-8F7C-71C46EBB9603}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="580" windowWidth="27040" windowHeight="15540" xr2:uid="{75E0E992-E93C-194B-84F3-B52702DB8E82}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="61">
   <si>
     <t>日期</t>
   </si>
@@ -180,6 +180,45 @@
   </si>
   <si>
     <t>午睡</t>
+  </si>
+  <si>
+    <t>当尼采哭泣 9-10 章</t>
+  </si>
+  <si>
+    <t>保龄球</t>
+  </si>
+  <si>
+    <t>学习</t>
+  </si>
+  <si>
+    <t>causality</t>
+  </si>
+  <si>
+    <t>youtube</t>
+  </si>
+  <si>
+    <t>当尼采哭泣</t>
+  </si>
+  <si>
+    <t>拉伸</t>
+  </si>
+  <si>
+    <t>午休</t>
+  </si>
+  <si>
+    <t>calibration</t>
+  </si>
+  <si>
+    <t>洗漱</t>
+  </si>
+  <si>
+    <t>研究视频</t>
+  </si>
+  <si>
+    <t>工资</t>
+  </si>
+  <si>
+    <t>检查条款</t>
   </si>
 </sst>
 </file>
@@ -541,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71202AD9-F6AE-7E4C-A4C7-3746B5A46B93}">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -973,7 +1012,7 @@
         <v>37</v>
       </c>
       <c r="D35" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1069,20 +1108,212 @@
       <c r="B43" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="C43" t="s">
+        <v>48</v>
+      </c>
+      <c r="D43" s="2">
+        <v>40</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>44949</v>
       </c>
+      <c r="B44" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" t="s">
+        <v>50</v>
+      </c>
+      <c r="D44" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>44949</v>
       </c>
+      <c r="B45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D45" s="2">
+        <v>30</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44949</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46" t="s">
+        <v>51</v>
+      </c>
+      <c r="D46" s="2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>44949</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D47" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>44950</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" t="s">
+        <v>53</v>
+      </c>
+      <c r="D49" s="2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>44950</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D50" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>44950</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D51" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>44950</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D52" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>44950</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C53" t="s">
+        <v>56</v>
+      </c>
+      <c r="D53" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>44951</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D55" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>44951</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C56" t="s">
+        <v>58</v>
+      </c>
+      <c r="D56" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>44951</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C57" t="s">
+        <v>60</v>
+      </c>
+      <c r="D57" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>44951</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" t="s">
+        <v>53</v>
+      </c>
+      <c r="D58" s="2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>44951</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D59" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>44951</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>44951</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>44951</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>44951</v>
       </c>
     </row>
   </sheetData>

</xml_diff>